<commit_message>
v0.6.6 - march 1st, 2025
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-alabama-consent-profile.xlsx
+++ b/docs/StructureDefinition-alabama-consent-profile.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.6.5</t>
+    <t>0.6.6</t>
   </si>
   <si>
     <t>Name</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-01-01T22:24:49-07:00</t>
+    <t>2025-03-01T21:28:29-06:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>